<commit_message>
improved ML algorithm. README new goals.
</commit_message>
<xml_diff>
--- a/electro.xlsx
+++ b/electro.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projekty\jupyter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27605361-301A-4FB9-A299-7E10EE99C2F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{54BA580A-31B8-451D-A683-240D3534D4F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A9889FAA-A050-48CC-B122-A61CEDCC1169}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A41D2436-7BD4-441F-89BD-40C3EE77A415}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="8">
   <si>
     <t>category</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>weak</t>
+  </si>
+  <si>
+    <t>TOYS</t>
+  </si>
+  <si>
+    <t>AGD</t>
   </si>
 </sst>
 </file>
@@ -412,15 +418,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9957E19-ED27-44B8-82EE-F8671FA52608}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAD1C07A-27C4-4425-B8D7-BCA2E8EFE7CD}">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="8.77734375" customWidth="1"/>
     <col min="2" max="2" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
@@ -436,8 +443,8 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>6</v>
       </c>
       <c r="B2" s="3">
         <v>1200</v>
@@ -447,8 +454,8 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
+      <c r="A3" t="s">
+        <v>7</v>
       </c>
       <c r="B3" s="3">
         <v>1200</v>
@@ -458,8 +465,8 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>2</v>
+      <c r="A4" t="s">
+        <v>7</v>
       </c>
       <c r="B4" s="3">
         <v>1000</v>
@@ -469,8 +476,8 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>2</v>
+      <c r="A5" t="s">
+        <v>7</v>
       </c>
       <c r="B5" s="3">
         <v>500</v>
@@ -480,8 +487,8 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>2</v>
+      <c r="A6" t="s">
+        <v>7</v>
       </c>
       <c r="B6" s="3">
         <v>200</v>
@@ -491,8 +498,8 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>1</v>
+      <c r="A7" t="s">
+        <v>6</v>
       </c>
       <c r="B7" s="3">
         <v>1500</v>
@@ -502,8 +509,8 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>1</v>
+      <c r="A8" t="s">
+        <v>6</v>
       </c>
       <c r="B8" s="3">
         <v>2000</v>
@@ -513,8 +520,8 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>1</v>
+      <c r="A9" t="s">
+        <v>6</v>
       </c>
       <c r="B9" s="3">
         <v>2500</v>
@@ -524,8 +531,8 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>1</v>
+      <c r="A10" t="s">
+        <v>6</v>
       </c>
       <c r="B10" s="3">
         <v>1700</v>
@@ -535,8 +542,8 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>1</v>
+      <c r="A11" t="s">
+        <v>6</v>
       </c>
       <c r="B11" s="3">
         <v>1000</v>
@@ -546,8 +553,8 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>1</v>
+      <c r="A12" t="s">
+        <v>6</v>
       </c>
       <c r="B12" s="3">
         <v>2500</v>
@@ -557,8 +564,8 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>1</v>
+      <c r="A13" t="s">
+        <v>6</v>
       </c>
       <c r="B13" s="3">
         <v>5000</v>
@@ -568,8 +575,8 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>1</v>
+      <c r="A14" t="s">
+        <v>6</v>
       </c>
       <c r="B14" s="3">
         <v>650</v>
@@ -579,8 +586,8 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>1</v>
+      <c r="A15" t="s">
+        <v>6</v>
       </c>
       <c r="B15" s="3">
         <v>100</v>
@@ -590,8 +597,8 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>1</v>
+      <c r="A16" t="s">
+        <v>6</v>
       </c>
       <c r="B16" s="3">
         <v>199</v>
@@ -601,8 +608,8 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>1</v>
+      <c r="A17" t="s">
+        <v>6</v>
       </c>
       <c r="B17" s="3">
         <v>149</v>
@@ -612,8 +619,8 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>1</v>
+      <c r="A18" t="s">
+        <v>6</v>
       </c>
       <c r="B18" s="3">
         <v>6000</v>
@@ -623,8 +630,8 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>1</v>
+      <c r="A19" t="s">
+        <v>6</v>
       </c>
       <c r="B19" s="3">
         <v>3500</v>
@@ -634,8 +641,8 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>1</v>
+      <c r="A20" t="s">
+        <v>6</v>
       </c>
       <c r="B20" s="3">
         <v>3900</v>
@@ -645,8 +652,8 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>1</v>
+      <c r="A21" t="s">
+        <v>6</v>
       </c>
       <c r="B21" s="3">
         <v>4150</v>
@@ -656,8 +663,8 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>1</v>
+      <c r="A22" t="s">
+        <v>6</v>
       </c>
       <c r="B22" s="3">
         <v>2900</v>
@@ -667,8 +674,8 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>1</v>
+      <c r="A23" t="s">
+        <v>6</v>
       </c>
       <c r="B23" s="3">
         <v>550</v>
@@ -678,8 +685,8 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <v>1</v>
+      <c r="A24" t="s">
+        <v>6</v>
       </c>
       <c r="B24" s="3">
         <v>127</v>
@@ -689,8 +696,8 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>1</v>
+      <c r="A25" t="s">
+        <v>6</v>
       </c>
       <c r="B25" s="3">
         <v>69</v>
@@ -700,8 +707,8 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>1</v>
+      <c r="A26" t="s">
+        <v>6</v>
       </c>
       <c r="B26" s="3">
         <v>1770</v>
@@ -711,8 +718,8 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <v>1</v>
+      <c r="A27" t="s">
+        <v>6</v>
       </c>
       <c r="B27" s="3">
         <v>1396</v>
@@ -722,8 +729,8 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28">
-        <v>1</v>
+      <c r="A28" t="s">
+        <v>6</v>
       </c>
       <c r="B28" s="3">
         <v>1300</v>
@@ -733,8 +740,8 @@
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29">
-        <v>2</v>
+      <c r="A29" t="s">
+        <v>7</v>
       </c>
       <c r="B29" s="3">
         <v>1300</v>
@@ -744,8 +751,8 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30">
-        <v>2</v>
+      <c r="A30" t="s">
+        <v>7</v>
       </c>
       <c r="B30" s="3">
         <v>1100</v>
@@ -755,8 +762,8 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31">
-        <v>2</v>
+      <c r="A31" t="s">
+        <v>7</v>
       </c>
       <c r="B31" s="3">
         <v>699</v>
@@ -766,8 +773,8 @@
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32">
-        <v>2</v>
+      <c r="A32" t="s">
+        <v>7</v>
       </c>
       <c r="B32" s="3">
         <v>123</v>
@@ -777,8 +784,8 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33">
-        <v>2</v>
+      <c r="A33" t="s">
+        <v>7</v>
       </c>
       <c r="B33" s="3">
         <v>2100</v>
@@ -788,8 +795,8 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34">
-        <v>2</v>
+      <c r="A34" t="s">
+        <v>7</v>
       </c>
       <c r="B34" s="3">
         <v>3400</v>
@@ -799,8 +806,8 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35">
-        <v>2</v>
+      <c r="A35" t="s">
+        <v>7</v>
       </c>
       <c r="B35" s="3">
         <v>363</v>
@@ -810,8 +817,8 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36">
-        <v>2</v>
+      <c r="A36" t="s">
+        <v>7</v>
       </c>
       <c r="B36" s="3">
         <v>177</v>
@@ -821,8 +828,8 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37">
-        <v>2</v>
+      <c r="A37" t="s">
+        <v>7</v>
       </c>
       <c r="B37" s="3">
         <v>98</v>
@@ -832,8 +839,8 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38">
-        <v>2</v>
+      <c r="A38" t="s">
+        <v>7</v>
       </c>
       <c r="B38" s="3">
         <v>2999</v>
@@ -843,8 +850,8 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39">
-        <v>2</v>
+      <c r="A39" t="s">
+        <v>7</v>
       </c>
       <c r="B39" s="3">
         <v>1245</v>
@@ -854,8 +861,8 @@
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40">
-        <v>2</v>
+      <c r="A40" t="s">
+        <v>7</v>
       </c>
       <c r="B40" s="3">
         <v>750</v>
@@ -865,8 +872,8 @@
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41">
-        <v>2</v>
+      <c r="A41" t="s">
+        <v>7</v>
       </c>
       <c r="B41" s="3">
         <v>29</v>
@@ -876,8 +883,8 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42">
-        <v>2</v>
+      <c r="A42" t="s">
+        <v>7</v>
       </c>
       <c r="B42" s="3">
         <v>1</v>
@@ -887,8 +894,8 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43">
-        <v>1</v>
+      <c r="A43" t="s">
+        <v>6</v>
       </c>
       <c r="B43" s="3">
         <v>99</v>
@@ -898,8 +905,8 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44">
-        <v>1</v>
+      <c r="A44" t="s">
+        <v>6</v>
       </c>
       <c r="B44" s="3">
         <v>76</v>
@@ -909,8 +916,8 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45">
-        <v>1</v>
+      <c r="A45" t="s">
+        <v>6</v>
       </c>
       <c r="B45" s="3">
         <v>129</v>
@@ -920,8 +927,8 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46">
-        <v>1</v>
+      <c r="A46" t="s">
+        <v>6</v>
       </c>
       <c r="B46" s="3">
         <v>29</v>
@@ -931,8 +938,8 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47">
-        <v>2</v>
+      <c r="A47" t="s">
+        <v>7</v>
       </c>
       <c r="B47" s="3">
         <v>44</v>
@@ -942,8 +949,8 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48">
-        <v>2</v>
+      <c r="A48" t="s">
+        <v>7</v>
       </c>
       <c r="B48" s="3">
         <v>888</v>
@@ -953,8 +960,8 @@
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49">
-        <v>2</v>
+      <c r="A49" t="s">
+        <v>7</v>
       </c>
       <c r="B49" s="3">
         <v>777</v>
@@ -964,8 +971,8 @@
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50">
-        <v>1</v>
+      <c r="A50" t="s">
+        <v>6</v>
       </c>
       <c r="B50" s="3">
         <v>2991</v>
@@ -975,8 +982,8 @@
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51">
-        <v>2</v>
+      <c r="A51" t="s">
+        <v>7</v>
       </c>
       <c r="B51" s="3">
         <v>66</v>

</xml_diff>